<commit_message>
Complete Lab 4 tasks a, b, c
</commit_message>
<xml_diff>
--- a/Lab Work/Lab 04 28.02.25/Bike_Sales_2021.xlsx
+++ b/Lab Work/Lab 04 28.02.25/Bike_Sales_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patti\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ME-402-Data-Analytics-Essentials\Lab Work\Lab 04 28.02.25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DB9CA61-6AE6-44E6-A916-5DC4888ED7F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D77F167-EDD3-4A7B-B93D-87342191DE89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="8964" xr2:uid="{D492E576-0D9E-4FBB-A74E-3E9FD5C50F25}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D492E576-0D9E-4FBB-A74E-3E9FD5C50F25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -223,7 +226,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -260,12 +263,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -285,9 +288,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -325,7 +328,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -431,7 +434,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -573,7 +576,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -583,31 +586,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FEBE038-5188-4BB3-A1EC-49FE8A6A2949}">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:R1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.90625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="12.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -663,7 +666,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>44227</v>
       </c>
@@ -722,7 +725,7 @@
         <v>33600</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>44255</v>
       </c>
@@ -781,7 +784,7 @@
         <v>71560</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>44286</v>
       </c>
@@ -840,7 +843,7 @@
         <v>24430</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>44316</v>
       </c>
@@ -899,7 +902,7 @@
         <v>22950</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>44347</v>
       </c>
@@ -947,18 +950,17 @@
       </c>
       <c r="P6" s="2">
         <f t="shared" si="0"/>
-        <v>2156</v>
+        <v>-24060</v>
       </c>
       <c r="Q6" s="2">
-        <f t="shared" si="1"/>
-        <v>3784</v>
+        <v>30000</v>
       </c>
       <c r="R6" s="2">
         <f t="shared" si="2"/>
         <v>5940</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>44377</v>
       </c>
@@ -1017,7 +1019,7 @@
         <v>15680</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>44408</v>
       </c>
@@ -1076,7 +1078,7 @@
         <v>73290</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>44439</v>
       </c>
@@ -1135,7 +1137,7 @@
         <v>15680</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>44469</v>
       </c>
@@ -1194,7 +1196,7 @@
         <v>13440</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>44500</v>
       </c>
@@ -1253,7 +1255,7 @@
         <v>91800</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>44530</v>
       </c>
@@ -1312,7 +1314,7 @@
         <v>168166</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>44561</v>
       </c>
@@ -1371,7 +1373,7 @@
         <v>17280</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>44592</v>
       </c>
@@ -1673,15 +1675,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="6cf0ffbd-cd96-4ba4-bd4f-bd34e8409846">
@@ -1700,14 +1693,49 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{638E245F-5B7F-4B70-A514-532F2327F29A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{638E245F-5B7F-4B70-A514-532F2327F29A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6cf0ffbd-cd96-4ba4-bd4f-bd34e8409846"/>
+    <ds:schemaRef ds:uri="ef7ae401-bd17-41a5-97cb-ef653218410e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28DA1A21-031B-42A7-AAD2-F764216F51B4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E448CC1-7C21-4F51-9E61-B31CDCD807B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6cf0ffbd-cd96-4ba4-bd4f-bd34e8409846"/>
+    <ds:schemaRef ds:uri="ef7ae401-bd17-41a5-97cb-ef653218410e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E448CC1-7C21-4F51-9E61-B31CDCD807B7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28DA1A21-031B-42A7-AAD2-F764216F51B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>